<commit_message>
update to use dictionaries and lists
</commit_message>
<xml_diff>
--- a/cities.xlsx
+++ b/cities.xlsx
@@ -11,52 +11,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>City</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
     <t>Solta</t>
   </si>
   <si>
+    <t>Croatia</t>
+  </si>
+  <si>
     <t>Greenville</t>
   </si>
   <si>
+    <t>USA</t>
+  </si>
+  <si>
     <t>Buenos Aires</t>
   </si>
   <si>
+    <t>Argentina</t>
+  </si>
+  <si>
     <t>Los Cabos</t>
   </si>
   <si>
+    <t>Mexico</t>
+  </si>
+  <si>
     <t>Walla Walla Valley</t>
   </si>
   <si>
     <t>Marakesh</t>
   </si>
   <si>
+    <t>Morocco</t>
+  </si>
+  <si>
     <t>Albuquerque</t>
   </si>
   <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
     <t>Archipelago Sea</t>
   </si>
   <si>
+    <t>Finland</t>
+  </si>
+  <si>
     <t>Iguazu Falls</t>
   </si>
   <si>
     <t>Salina Island</t>
   </si>
   <si>
+    <t>Italy</t>
+  </si>
+  <si>
     <t>Toronto</t>
   </si>
   <si>
+    <t>Canada</t>
+  </si>
+  <si>
     <t>Pyeongchang</t>
+  </si>
+  <si>
+    <t>South Korea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -67,9 +106,15 @@
       <color rgb="FF000000"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF222222"/>
+      <name val="Sans-serif"/>
     </font>
   </fonts>
   <fills count="3">
@@ -92,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -101,6 +146,18 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -120,119 +177,234 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="17.43"/>
+    <col customWidth="1" min="4" max="4" width="24.0"/>
+  </cols>
   <sheetData>
     <row r="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" ht="17.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" ht="17.25">
-      <c r="A3" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" ht="17.25">
-      <c r="A4" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" ht="17.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" ht="17.25">
-      <c r="A6" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" ht="17.25">
-      <c r="A7" s="1" t="s">
+      <c r="C2" s="2">
+        <v>1700.0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" ht="17.25">
-      <c r="A8" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" ht="17.25">
-      <c r="A9" s="1" t="s">
+      <c r="C3" s="2">
+        <v>84554.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>68.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" ht="17.25">
-      <c r="A10" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" ht="17.25">
-      <c r="A11" s="1" t="s">
+      <c r="C4" s="2">
+        <v>1.3591863E7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4758.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" ht="17.25">
-      <c r="A12" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" ht="17.25">
-      <c r="A13" s="1" t="s">
+      <c r="C5" s="2">
+        <v>287651.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3750.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>32237.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>928850.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>559277.0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>491.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <v>60000.0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8300.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>672.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4000.0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2">
+        <v>630.0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2731571.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2581000.0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3194.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="6"/>
     </row>
     <row r="20">
-      <c r="A20" s="2"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
     </row>
     <row r="26">
-      <c r="A26" s="2"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27">
-      <c r="A27" s="2"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28">
-      <c r="A28" s="2"/>
+      <c r="A28" s="3"/>
     </row>
     <row r="29">
-      <c r="A29" s="2"/>
+      <c r="A29" s="3"/>
     </row>
     <row r="30">
-      <c r="A30" s="2"/>
+      <c r="A30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="2"/>
+      <c r="A31" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>